<commit_message>
All tests modified (DB connection added) + PERFORM_LONG_UI_CHECKS added
</commit_message>
<xml_diff>
--- a/addressbook-web-tests/addressbook-web-tests/groups.xlsx
+++ b/addressbook-web-tests/addressbook-web-tests/groups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\csharp_training\addressbook-web-tests\addressbook-test-data-generators\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\csharp_training\addressbook-web-tests\addressbook-web-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,9 +29,6 @@
     <t>_Z</t>
   </si>
   <si>
-    <t>?`2'Q*</t>
-  </si>
-  <si>
     <t>-YQ</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>H/8GP\</t>
+  </si>
+  <si>
+    <t>?2Q*</t>
   </si>
 </sst>
 </file>
@@ -380,32 +380,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>